<commit_message>
Small changes in test cases and bug report.
</commit_message>
<xml_diff>
--- a/Test_cases_Bug_report/Test cases.xlsx
+++ b/Test_cases_Bug_report/Test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alza\Test_cases_Bug_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D4CB4C-80D7-4BD0-B76B-F309846C6EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAFD33E-8E89-48AB-8514-F112DA066F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,31 +300,6 @@
     <t>Item is removed from watchdogs, there is text "Vaše bouda s hlídacími psy je prázdná." displayed.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Title:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Account changes</t>
-    </r>
-  </si>
-  <si>
     <t>Go to account settings by clicking "Moje Alza - wedey95103@haizail.com" in top menu. Then "Nastavení účtu" - "Můj účet".</t>
   </si>
   <si>
@@ -817,6 +792,31 @@
   </si>
   <si>
     <t>Account settings page displayed, fields "Ulice", "PSČ" and "Město" have values provided into them.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Title:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+User account changes</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1277,7 +1277,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,7 +1575,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="5" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -1633,10 +1633,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -1689,7 +1689,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1703,7 +1703,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1787,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80E4BF2-6951-4AE4-AF22-3AF40F2E413B}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -1863,10 +1863,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1901,7 +1901,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2001,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6626145F-A1D0-4F8A-953A-E0E6694FE922}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="5" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2077,10 +2077,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2195,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB03449A-6CFC-4A50-AB52-2DB802D624F4}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2271,10 +2271,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2309,7 +2309,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
@@ -2339,7 +2339,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -2365,7 +2365,7 @@
         <v>100</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -2385,11 +2385,11 @@
         <v>10</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2397,11 +2397,11 @@
         <v>11</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2447,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC8B5FD-24F7-4D4A-8252-558FC277C5A5}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2459,7 +2459,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="2" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="3" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2523,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
@@ -2575,11 +2575,11 @@
         <v>5</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2587,13 +2587,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2601,11 +2601,11 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2613,11 +2613,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2625,11 +2625,11 @@
         <v>9</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added assertion at watchdogs.
</commit_message>
<xml_diff>
--- a/Test_cases_Bug_report/Test cases.xlsx
+++ b/Test_cases_Bug_report/Test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alza\Test_cases_Bug_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAFD33E-8E89-48AB-8514-F112DA066F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5D2880-91D6-4C8D-B135-24C614433D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,282 +553,291 @@
     <t>Dialog disappears.</t>
   </si>
   <si>
+    <t>Remove item from watchdogs by clicking both checkboxes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 - Critical</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 - High</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 - Medium</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Related user story:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+As a user I can log into Alza webpage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Related user story:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+As a user I can put and remove items from basket at Alza webpage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Related user story:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+As a user I can perform search at Alza webpage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Related user story:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+As a user I can set watchdog to an item and remove it at Alza webpage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Related user story:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+As a user I can change my account at Alza webpage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Title:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Login, logout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to Alza</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> webpage</t>
+    </r>
+  </si>
+  <si>
+    <t>Account settings page displayed, fields "Ulice", "PSČ" and "Město" have values provided into them.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Title:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+User account changes</t>
+    </r>
+  </si>
+  <si>
     <t>Watchdogs page is displayed with:
 1) Item at which "Hlídat cenu" was clicked.
 2) Two checkboxes for watching price and availability.
+3) At the checkbox for watching price there is a price limit displayed that was provided.
 Note:
 There is also ohter stuff displayed like most watched products, etc.</t>
-  </si>
-  <si>
-    <t>Remove item from watchdogs by clicking both checkboxes.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 - Critical</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2 - High</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3 - Medium</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Related user story:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-As a user I can log into Alza webpage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Related user story:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-As a user I can put and remove items from basket at Alza webpage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Related user story:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-As a user I can perform search at Alza webpage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Related user story:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-As a user I can set watchdog to an item and remove it at Alza webpage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Related user story:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-As a user I can change my account at Alza webpage</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Title:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Login, logout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to Alza</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> webpage</t>
-    </r>
-  </si>
-  <si>
-    <t>Account settings page displayed, fields "Ulice", "PSČ" and "Město" have values provided into them.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Title:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-User account changes</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1159,7 +1168,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1184,100 +1193,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1575,7 +1584,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1599,7 +1608,7 @@
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -1607,7 +1616,7 @@
     </row>
     <row r="5" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -1823,7 +1832,7 @@
     </row>
     <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -1831,7 +1840,7 @@
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2037,7 +2046,7 @@
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -2045,7 +2054,7 @@
     </row>
     <row r="5" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2231,7 +2240,7 @@
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -2239,7 +2248,7 @@
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2362,7 +2371,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>65</v>
@@ -2380,7 +2389,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>10</v>
       </c>
@@ -2389,7 +2398,7 @@
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="18" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2397,7 +2406,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="18" t="s">
@@ -2459,7 +2468,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -2483,7 +2492,7 @@
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -2491,7 +2500,7 @@
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2617,7 +2626,7 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">

</xml_diff>